<commit_message>
Minor changes after major change in prev commit
</commit_message>
<xml_diff>
--- a/Group Allocator.xlsx
+++ b/Group Allocator.xlsx
@@ -17,6 +17,16 @@
     <sheet name="StudentDataEntry" sheetId="3" r:id="rId3"/>
     <sheet name="GroupList" sheetId="27" r:id="rId4"/>
     <sheet name="SummaryResults" sheetId="7" r:id="rId5"/>
+    <sheet name="g_GPA" sheetId="89" r:id="rId6"/>
+    <sheet name="g_Gender" sheetId="90" r:id="rId7"/>
+    <sheet name="g_A_spec" sheetId="91" r:id="rId8"/>
+    <sheet name="g_B_spec" sheetId="92" r:id="rId9"/>
+    <sheet name="g_C_spec" sheetId="93" r:id="rId10"/>
+    <sheet name="g_A_eth" sheetId="94" r:id="rId11"/>
+    <sheet name="g_B_eth" sheetId="95" r:id="rId12"/>
+    <sheet name="g_C_eth" sheetId="96" r:id="rId13"/>
+    <sheet name="g_D_eth" sheetId="97" r:id="rId14"/>
+    <sheet name="g_E_eth" sheetId="98" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="ethnicity" localSheetId="2">OFFSET(StudentDataEntry!$F$2,0,0,COUNTA(StudentDataEntry!$A:$A)-1,1)</definedName>
@@ -1048,6 +1058,21 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Mean GPA and Variance of GPA</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
@@ -1204,6 +1229,152 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>GPA Variance</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>SummaryResults!$D$2:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>SummaryResults!$I$2:$I$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>4.4947451872515192</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.4246136773399209</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.9326139607311803</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.9754603759204672</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.3049433611648427</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.6736652773919274</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.9919316820726118</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.7136610203278932</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.7242057261132846</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.6927527738975123</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.5072459691161693</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.2471597279499678</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.2161681268272142</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.9094174424781802</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.9325698450729472</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.1157628977435685</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.0549417456923189</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.9685067402172325</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.934226391113353</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.3261673319380938</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1213,21 +1384,40 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="849795728"/>
-        <c:axId val="723591808"/>
+        <c:axId val="849764760"/>
+        <c:axId val="849793768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="849795728"/>
+        <c:axId val="849764760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Group</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="723591808"/>
+        <c:crossAx val="849793768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1235,24 +1425,45 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="723591808"/>
+        <c:axId val="849793768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="9"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>GPA</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="849795728"/>
+        <c:crossAx val="849764760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="t"/>
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
@@ -1260,12 +1471,2828 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Number of E in each group</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>E</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>SummaryResults!$D$2:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>SummaryResults!$Q$2:$Q$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="717453968"/>
+        <c:axId val="717447696"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="717453968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Group</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="717447696"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="717447696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="27"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Number of Students</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="717453968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Number of Males and Females in each group</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Male</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>SummaryResults!$D$2:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>SummaryResults!$F$2:$F$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Female</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>SummaryResults!$D$2:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>SummaryResults!$G$2:$G$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="491850800"/>
+        <c:axId val="324041376"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="491850800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Group</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="324041376"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="324041376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="27"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Number of Students</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="491850800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Number from A in each group</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>A</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>SummaryResults!$D$2:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>SummaryResults!$J$2:$J$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="393434472"/>
+        <c:axId val="393436432"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="393434472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Group</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="393436432"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="393436432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="27"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Number of Students</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="393434472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Number from B in each group</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>B</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>SummaryResults!$D$2:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>SummaryResults!$K$2:$K$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="723585144"/>
+        <c:axId val="392724800"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="723585144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Group</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="392724800"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="392724800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="27"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Number of Students</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="723585144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Number from C in each group</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>C</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>SummaryResults!$D$2:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>SummaryResults!$L$2:$L$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="929723224"/>
+        <c:axId val="929723616"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="929723224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Group</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="929723616"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="929723616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="27"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Number of Students</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="929723224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Number of A in each group</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>A</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>SummaryResults!$D$2:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>SummaryResults!$M$2:$M$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="929727144"/>
+        <c:axId val="929725184"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="929727144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Group</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="929725184"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="929725184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="27"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Number of Students</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="929727144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Number of B in each group</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>B</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>SummaryResults!$D$2:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>SummaryResults!$N$2:$N$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="929738120"/>
+        <c:axId val="849768680"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="929738120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Group</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="849768680"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="849768680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="27"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Number of Students</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="929738120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Number of C in each group</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>C</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>SummaryResults!$D$2:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>SummaryResults!$O$2:$O$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="717437112"/>
+        <c:axId val="717440248"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="717437112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Group</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="717440248"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="717440248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="27"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Number of Students</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="717437112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Number of D in each group</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>D</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>SummaryResults!$D$2:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>SummaryResults!$P$2:$P$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="717439072"/>
+        <c:axId val="717441816"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="717439072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Group</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="717441816"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="717441816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="27"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Number of Students</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="717439072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="179" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="179" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="179" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="179" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="179" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="179" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="179" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="179" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="179" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="179" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1651,25 +4678,17 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8668282" cy="6295014"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="63" name="Chart 62"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1682,7 +4701,250 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8668282" cy="6295014"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8668282" cy="6295014"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8668282" cy="6295014"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8668282" cy="6295014"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8668282" cy="6295014"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8668282" cy="6295014"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8668282" cy="6295014"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8668282" cy="6295014"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8668282" cy="6295014"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2669,7 +5931,7 @@
   <dimension ref="A1:O501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20415,7 +23677,7 @@
   <dimension ref="A1:AE21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21455,8 +24717,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -21825,6 +25086,7 @@
     a.FullSeriesCollection(1).Name = "Male"
     a.FullSeriesCollection(1).Values = ws.Range(ws.Cells(2, 6), ws.Cells(1 + number_groups, 6))
     a.FullSeriesCollection(1).XValues = x_axis_range
+    a.SeriesCollection().NewSeries()
     a.FullSeriesCollection(2).Name = "Female"
     a.FullSeriesCollection(2).Values = ws.Range(ws.Cells(2, 7), ws.Cells(1 + number_groups, 7))
     a.FullSeriesCollection(2).XValues = x_axis_range
@@ -21971,7 +25233,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69CC30D7-0C23-48A7-94B6-D3425D793938}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9538018-61DB-48A9-8C79-BCD108C72C60}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://opensolver.org"/>

</xml_diff>